<commit_message>
Adicionado mapa de memoria
</commit_message>
<xml_diff>
--- a/Mapa de Memoria/Memoria 24C1025 da Placa Mãe - Destinada principalmente à FAT 8.xlsx
+++ b/Mapa de Memoria/Memoria 24C1025 da Placa Mãe - Destinada principalmente à FAT 8.xlsx
@@ -366,11 +366,11 @@
   <dimension ref="A1:Q1066"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7547" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V7641" activeCellId="0" sqref="V7641"/>
+      <selection pane="bottomLeft" activeCell="A7547" activeCellId="0" sqref="A7547"/>
+      <selection pane="bottomRight" activeCell="P7410" activeCellId="0" sqref="P7410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26353,6 +26353,554 @@
     <row r="7642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7776" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7784" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7785" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7804" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7823" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7835" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7836" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7847" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7853" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7860" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7867" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7868" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7869" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7870" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7871" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7872" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7873" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7874" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7875" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7876" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7877" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7878" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7879" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7930" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7934" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7935" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7936" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7939" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7940" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7941" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7942" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7943" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7944" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7945" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7946" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7947" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7948" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7949" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7950" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7951" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7952" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7953" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7954" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7959" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7963" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7965" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7968" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7973" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7976" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7980" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8000" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8009" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8010" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8011" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8012" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8013" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8014" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8015" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8016" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8017" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8018" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8019" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8020" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8021" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8022" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8023" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8024" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8025" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8026" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8027" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8028" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8029" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8033" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8034" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8035" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8036" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8037" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8038" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8039" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8040" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8041" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8042" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8043" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8044" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8045" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8046" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8047" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8048" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8049" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8050" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8051" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8053" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8054" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8055" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8056" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8057" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8058" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8059" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8060" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8061" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8062" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8063" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8064" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8065" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8066" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8067" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8068" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8069" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8070" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8071" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8072" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8073" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8074" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8075" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8076" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8077" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8078" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8079" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8080" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8081" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8082" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8083" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8084" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8085" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8086" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8087" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8088" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8089" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8090" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8091" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8092" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8093" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8094" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8095" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8096" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8097" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8098" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8099" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>